<commit_message>
added Boston, Dallas, Boulder, Chicago
</commit_message>
<xml_diff>
--- a/Data/Specific Power Plots for Reactor Scale_bk_12.19.22.xlsx
+++ b/Data/Specific Power Plots for Reactor Scale_bk_12.19.22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atpha\Documents\Postdocs\Projects\TES\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF8E2A7-2DAC-44CC-B873-3D4647E849A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59445A50-ED5E-4508-A809-E037B21689C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" firstSheet="1" activeTab="2" xr2:uid="{CCAFE77B-233B-4F54-892D-EC466BD3AAF1}"/>
+    <workbookView xWindow="4395" yWindow="2535" windowWidth="21600" windowHeight="11055" xr2:uid="{CCAFE77B-233B-4F54-892D-EC466BD3AAF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Constant_power" sheetId="2" r:id="rId1"/>
@@ -7300,16 +7300,21 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.59765625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -7335,7 +7340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -7356,7 +7361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0.98989898989898994</v>
       </c>
@@ -7377,7 +7382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0.97979797979798</v>
       </c>
@@ -7398,7 +7403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0.96969696969696995</v>
       </c>
@@ -7419,7 +7424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0.95959595959596</v>
       </c>
@@ -7440,7 +7445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0.94949494949494995</v>
       </c>
@@ -7461,7 +7466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0.939393939393939</v>
       </c>
@@ -7482,7 +7487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0.92929292929292895</v>
       </c>
@@ -7503,7 +7508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0.919191919191919</v>
       </c>
@@ -7524,7 +7529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>0.90909090909090895</v>
       </c>
@@ -7545,7 +7550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0.89898989898989901</v>
       </c>
@@ -7566,7 +7571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0.88888888888888895</v>
       </c>
@@ -7587,7 +7592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0.87878787878787901</v>
       </c>
@@ -7608,7 +7613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>0.86868686868686895</v>
       </c>
@@ -7629,7 +7634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0.85858585858585901</v>
       </c>
@@ -7650,7 +7655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0.84848484848484895</v>
       </c>
@@ -7671,7 +7676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>0.83838383838383801</v>
       </c>
@@ -7692,7 +7697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0.82828282828282795</v>
       </c>
@@ -7713,7 +7718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>0.81818181818181801</v>
       </c>
@@ -7734,7 +7739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>0.80808080808080796</v>
       </c>
@@ -7755,7 +7760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>0.79797979797979801</v>
       </c>
@@ -7776,7 +7781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>0.78787878787878796</v>
       </c>
@@ -7797,7 +7802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>0.77777777777777801</v>
       </c>
@@ -7818,7 +7823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>0.76767676767676796</v>
       </c>
@@ -7839,7 +7844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>0.75757575757575801</v>
       </c>
@@ -7860,7 +7865,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>0.74747474747474696</v>
       </c>
@@ -7881,7 +7886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>0.73737373737373701</v>
       </c>
@@ -7902,7 +7907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>0.72727272727272696</v>
       </c>
@@ -7923,7 +7928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>0.71717171717171702</v>
       </c>
@@ -7944,7 +7949,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>0.70707070707070696</v>
       </c>
@@ -7965,7 +7970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0.69696969696969702</v>
       </c>
@@ -7986,7 +7991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>0.68686868686868696</v>
       </c>
@@ -8007,7 +8012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>0.67676767676767702</v>
       </c>
@@ -8028,7 +8033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>0.66666666666666696</v>
       </c>
@@ -8049,7 +8054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>0.65656565656565702</v>
       </c>
@@ -8070,7 +8075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>0.64646464646464596</v>
       </c>
@@ -8091,7 +8096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>0.63636363636363602</v>
       </c>
@@ -8112,7 +8117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>0.62626262626262597</v>
       </c>
@@ -8133,7 +8138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>0.61616161616161602</v>
       </c>
@@ -8154,7 +8159,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>0.60606060606060597</v>
       </c>
@@ -8175,7 +8180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>0.59595959595959602</v>
       </c>
@@ -8196,7 +8201,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>0.58585858585858597</v>
       </c>
@@ -8217,7 +8222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>0.57575757575757602</v>
       </c>
@@ -8238,7 +8243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>0.56565656565656597</v>
       </c>
@@ -8259,7 +8264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>0.55555555555555602</v>
       </c>
@@ -8280,7 +8285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>0.54545454545454497</v>
       </c>
@@ -8301,7 +8306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>0.53535353535353503</v>
       </c>
@@ -8322,7 +8327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>0.52525252525252497</v>
       </c>
@@ -8343,7 +8348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>0.51515151515151503</v>
       </c>
@@ -8364,7 +8369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>0.50505050505050497</v>
       </c>
@@ -8385,7 +8390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>0.49494949494949497</v>
       </c>
@@ -8406,7 +8411,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>0.48484848484848497</v>
       </c>
@@ -8427,7 +8432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>0.47474747474747497</v>
       </c>
@@ -8448,7 +8453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>0.46464646464646497</v>
       </c>
@@ -8469,7 +8474,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>0.45454545454545497</v>
       </c>
@@ -8490,7 +8495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>0.44444444444444398</v>
       </c>
@@ -8511,7 +8516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>0.43434343434343398</v>
       </c>
@@ -8532,7 +8537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>0.42424242424242398</v>
       </c>
@@ -8553,7 +8558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>0.41414141414141398</v>
       </c>
@@ -8574,7 +8579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>0.40404040404040398</v>
       </c>
@@ -8595,7 +8600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>0.39393939393939398</v>
       </c>
@@ -8616,7 +8621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>0.38383838383838398</v>
       </c>
@@ -8637,7 +8642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>0.37373737373737398</v>
       </c>
@@ -8658,7 +8663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>0.36363636363636398</v>
       </c>
@@ -8679,7 +8684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>0.35353535353535398</v>
       </c>
@@ -8700,7 +8705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>0.34343434343434298</v>
       </c>
@@ -8721,7 +8726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>0.33333333333333298</v>
       </c>
@@ -8742,7 +8747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>0.32323232323232298</v>
       </c>
@@ -8763,7 +8768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>0.31313131313131298</v>
       </c>
@@ -8784,7 +8789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>0.30303030303030298</v>
       </c>
@@ -8805,7 +8810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>0.29292929292929298</v>
       </c>
@@ -8826,7 +8831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>0.28282828282828298</v>
       </c>
@@ -8847,7 +8852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>0.27272727272727298</v>
       </c>
@@ -8868,7 +8873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>0.26262626262626299</v>
       </c>
@@ -8889,7 +8894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>0.25252525252525299</v>
       </c>
@@ -8910,7 +8915,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>0.24242424242424199</v>
       </c>
@@ -8931,7 +8936,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>0.23232323232323199</v>
       </c>
@@ -8952,7 +8957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>0.22222222222222199</v>
       </c>
@@ -8973,7 +8978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>0.21212121212121199</v>
       </c>
@@ -8994,7 +8999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>0.20202020202020199</v>
       </c>
@@ -9015,7 +9020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>0.19191919191919199</v>
       </c>
@@ -9036,7 +9041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>0.18181818181818199</v>
       </c>
@@ -9057,7 +9062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>0.17171717171717199</v>
       </c>
@@ -9078,7 +9083,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>0.16161616161616199</v>
       </c>
@@ -9099,7 +9104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>0.15151515151515199</v>
       </c>
@@ -9120,7 +9125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>0.14141414141414099</v>
       </c>
@@ -9141,7 +9146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>0.13131313131313099</v>
       </c>
@@ -9162,7 +9167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>0.12121212121212099</v>
       </c>
@@ -9183,7 +9188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>0.11111111111111099</v>
       </c>
@@ -9204,7 +9209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>0.10101010101010099</v>
       </c>
@@ -9225,7 +9230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>9.0909090909090898E-2</v>
       </c>
@@ -9246,7 +9251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>8.0808080808080801E-2</v>
       </c>
@@ -9267,7 +9272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>7.0707070707070704E-2</v>
       </c>
@@ -9288,7 +9293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>6.0606060606060601E-2</v>
       </c>
@@ -9309,7 +9314,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>5.0505050505050497E-2</v>
       </c>
@@ -9330,7 +9335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>4.0404040404040401E-2</v>
       </c>
@@ -9351,7 +9356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>3.03030303030303E-2</v>
       </c>
@@ -9372,7 +9377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>2.02020202020202E-2</v>
       </c>
@@ -9393,7 +9398,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>1.01010101010101E-2</v>
       </c>
@@ -9414,7 +9419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>0</v>
       </c>
@@ -9447,12 +9452,15 @@
   <dimension ref="A1:B129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="61.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9460,7 +9468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9468,7 +9476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.99985000000000002</v>
       </c>
@@ -9476,7 +9484,7 @@
         <v>8.7837837837813151</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.99972000000000005</v>
       </c>
@@ -9484,7 +9492,7 @@
         <v>8.7837837837813151</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.99958999999999998</v>
       </c>
@@ -9492,7 +9500,7 @@
         <v>8.7837837837888166</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.99946000000000002</v>
       </c>
@@ -9500,7 +9508,7 @@
         <v>8.7837837837813151</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.99933000000000005</v>
       </c>
@@ -9508,7 +9516,7 @@
         <v>8.7837837837813151</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.99919000000000002</v>
       </c>
@@ -9516,7 +9524,7 @@
         <v>9.4594594594614172</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.99905999999999995</v>
       </c>
@@ -9524,7 +9532,7 @@
         <v>8.7837837837888166</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.99892999999999998</v>
       </c>
@@ -9532,7 +9540,7 @@
         <v>8.7837837837813151</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.99878999999999996</v>
       </c>
@@ -9540,7 +9548,7 @@
         <v>9.4594594594614172</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.99865999999999999</v>
       </c>
@@ -9548,7 +9556,7 @@
         <v>8.7837837837813151</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.99851999999999996</v>
       </c>
@@ -9556,7 +9564,7 @@
         <v>9.4594594594614172</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.99839</v>
       </c>
@@ -9564,7 +9572,7 @@
         <v>8.7837837837813151</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.99824999999999997</v>
       </c>
@@ -9572,7 +9580,7 @@
         <v>9.4594594594614172</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.99812000000000001</v>
       </c>
@@ -9580,7 +9588,7 @@
         <v>8.7837837837813151</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.99797999999999998</v>
       </c>
@@ -9588,7 +9596,7 @@
         <v>9.4594594594614172</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.99783999999999995</v>
       </c>
@@ -9596,7 +9604,7 @@
         <v>9.4594594594614172</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.99770000000000003</v>
       </c>
@@ -9604,7 +9612,7 @@
         <v>9.4594594594539174</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.99756</v>
       </c>
@@ -9612,7 +9620,7 @@
         <v>9.4594594594614172</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.99743000000000004</v>
       </c>
@@ -9620,7 +9628,7 @@
         <v>8.7837837837813151</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.99731000000000003</v>
       </c>
@@ -9628,7 +9636,7 @@
         <v>10.135135135135894</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.99589000000000005</v>
       </c>
@@ -9636,7 +9644,7 @@
         <v>9.5945945945944384</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.99443999999999999</v>
       </c>
@@ -9644,7 +9652,7 @@
         <v>9.7972972972977175</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.99297000000000002</v>
       </c>
@@ -9652,7 +9660,7 @@
         <v>9.9324324324322379</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.99148000000000003</v>
       </c>
@@ -9660,7 +9668,7 @@
         <v>10.067567567567508</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.99</v>
       </c>
@@ -9668,7 +9676,7 @@
         <v>10.000000000000249</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0.98851999999999995</v>
       </c>
@@ -9676,7 +9684,7 @@
         <v>10.000000000000249</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.98706000000000005</v>
       </c>
@@ -9684,7 +9692,7 @@
         <v>9.864864864864229</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.98560999999999999</v>
       </c>
@@ -9692,7 +9700,7 @@
         <v>9.7972972972977175</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.98419000000000001</v>
       </c>
@@ -9700,7 +9708,7 @@
         <v>9.5945945945944384</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.98277999999999999</v>
       </c>
@@ -9708,7 +9716,7 @@
         <v>9.5270270270271791</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.98138999999999998</v>
       </c>
@@ -9716,7 +9724,7 @@
         <v>9.3918918918919072</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.98001000000000005</v>
       </c>
@@ -9724,7 +9732,7 @@
         <v>9.3243243243238982</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.97863</v>
       </c>
@@ -9732,7 +9740,7 @@
         <v>9.3243243243246461</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0.97726999999999997</v>
       </c>
@@ -9740,7 +9748,7 @@
         <v>9.1891891891893778</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.97589999999999999</v>
       </c>
@@ -9748,7 +9756,7 @@
         <v>9.2567567567566371</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.97453999999999996</v>
       </c>
@@ -9756,7 +9764,7 @@
         <v>9.1891891891893778</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0.97316999999999998</v>
       </c>
@@ -9764,7 +9772,7 @@
         <v>9.2567567567566371</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.97180999999999995</v>
       </c>
@@ -9772,7 +9780,7 @@
         <v>9.1891891891893778</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.97180999999999995</v>
       </c>
@@ -9780,7 +9788,7 @@
         <v>9.1891891891893778</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.94452000000000003</v>
       </c>
@@ -9788,7 +9796,7 @@
         <v>9.2195945945945699</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.9173</v>
       </c>
@@ -9796,7 +9804,7 @@
         <v>9.1959459459459527</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0.89015999999999995</v>
       </c>
@@ -9804,7 +9812,7 @@
         <v>9.1689189189189353</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.86312</v>
       </c>
@@ -9812,7 +9820,7 @@
         <v>9.1351351351351191</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.83620000000000005</v>
       </c>
@@ -9820,7 +9828,7 @@
         <v>9.0945945945945752</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0.80942999999999998</v>
       </c>
@@ -9828,7 +9836,7 @@
         <v>9.0439189189189424</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0.78283000000000003</v>
       </c>
@@ -9836,7 +9844,7 @@
         <v>8.9864864864864717</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0.75643000000000005</v>
       </c>
@@ -9844,7 +9852,7 @@
         <v>8.9189189189189122</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.73026999999999997</v>
       </c>
@@ -9852,7 +9860,7 @@
         <v>8.8378378378378617</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0.70438000000000001</v>
       </c>
@@ -9860,7 +9868,7 @@
         <v>8.7466216216216104</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0.67881999999999998</v>
       </c>
@@ -9868,7 +9876,7 @@
         <v>8.635135135135144</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0.65363000000000004</v>
       </c>
@@ -9876,7 +9884,7 @@
         <v>8.510135135135112</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0.62883</v>
       </c>
@@ -9884,7 +9892,7 @@
         <v>8.3783783783783932</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0.60448999999999997</v>
       </c>
@@ -9892,7 +9900,7 @@
         <v>8.2229729729729808</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>0.58062999999999998</v>
       </c>
@@ -9900,7 +9908,7 @@
         <v>8.060810810810807</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0.55728999999999995</v>
       </c>
@@ -9908,7 +9916,7 @@
         <v>7.885135135135144</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0.53451000000000004</v>
       </c>
@@ -9916,7 +9924,7 @@
         <v>7.6959459459459163</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>0.51229999999999998</v>
       </c>
@@ -9924,7 +9932,7 @@
         <v>7.5033783783784003</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>0.49070000000000003</v>
       </c>
@@ -9932,7 +9940,7 @@
         <v>7.2972972972972814</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0.46970000000000001</v>
       </c>
@@ -9940,7 +9948,7 @@
         <v>7.094594594594601</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0.44934000000000002</v>
       </c>
@@ -9948,7 +9956,7 @@
         <v>6.8783783783783736</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0.42959999999999998</v>
       </c>
@@ -9956,7 +9964,7 @@
         <v>6.6689189189189308</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0.41049999999999998</v>
       </c>
@@ -9964,7 +9972,7 @@
         <v>6.4527027027027053</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0.39202999999999999</v>
       </c>
@@ -9972,7 +9980,7 @@
         <v>6.2398648648648605</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0.37418000000000001</v>
       </c>
@@ -9980,7 +9988,7 @@
         <v>6.0304054054053973</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0.35694999999999999</v>
       </c>
@@ -9988,7 +9996,7 @@
         <v>5.8209459459459536</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0.34033000000000002</v>
       </c>
@@ -9996,7 +10004,7 @@
         <v>5.6148648648648543</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0.32429999999999998</v>
       </c>
@@ -10004,7 +10012,7 @@
         <v>5.4155405405405563</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0.30886000000000002</v>
       </c>
@@ -10012,7 +10020,7 @@
         <v>5.2162162162162007</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0.29398999999999997</v>
       </c>
@@ -10020,7 +10028,7 @@
         <v>5.0236486486486651</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0.27967999999999998</v>
       </c>
@@ -10028,7 +10036,7 @@
         <v>4.8344594594594552</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0.26591999999999999</v>
       </c>
@@ -10036,7 +10044,7 @@
         <v>4.6486486486486465</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0.25268000000000002</v>
       </c>
@@ -10044,7 +10052,7 @@
         <v>4.4729729729729639</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0.23995</v>
       </c>
@@ -10052,7 +10060,7 @@
         <v>4.3006756756756825</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0.22772999999999999</v>
       </c>
@@ -10060,7 +10068,7 @@
         <v>4.1283783783783816</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0.21598999999999999</v>
       </c>
@@ -10068,7 +10076,7 @@
         <v>3.9662162162162167</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0.20471</v>
       </c>
@@ -10076,7 +10084,7 @@
         <v>3.8108108108108056</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0.19389999999999999</v>
       </c>
@@ -10084,7 +10092,7 @@
         <v>3.6520270270270316</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>0.18351999999999999</v>
       </c>
@@ -10092,7 +10100,7 @@
         <v>3.506756756756757</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0.17357</v>
       </c>
@@ -10100,7 +10108,7 @@
         <v>3.361486486486482</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0.16403999999999999</v>
       </c>
@@ -10108,7 +10116,7 @@
         <v>3.2195945945945978</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0.15490999999999999</v>
       </c>
@@ -10116,7 +10124,7 @@
         <v>3.0844594594594592</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0.14616000000000001</v>
       </c>
@@ -10124,7 +10132,7 @@
         <v>2.9560810810810745</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0.13780000000000001</v>
       </c>
@@ -10132,7 +10140,7 @@
         <v>2.8243243243243268</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0.12978999999999999</v>
       </c>
@@ -10140,7 +10148,7 @@
         <v>2.7060810810810865</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0.12214</v>
       </c>
@@ -10148,7 +10156,7 @@
         <v>2.5844594594594557</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>0.11482000000000001</v>
       </c>
@@ -10156,7 +10164,7 @@
         <v>2.4729729729729706</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0.10784000000000001</v>
       </c>
@@ -10164,7 +10172,7 @@
         <v>2.3581081081081083</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0.10118000000000001</v>
       </c>
@@ -10172,7 +10180,7 @@
         <v>2.2499999999999996</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>9.4818E-2</v>
       </c>
@@ -10180,7 +10188,7 @@
         <v>2.1493243243243261</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>8.8759000000000005E-2</v>
       </c>
@@ -10188,7 +10196,7 @@
         <v>2.0469594594594573</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>8.2987000000000005E-2</v>
       </c>
@@ -10196,7 +10204,7 @@
         <v>1.9499999999999997</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>7.7493999999999993E-2</v>
       </c>
@@ -10204,7 +10212,7 @@
         <v>1.855743243243247</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>7.2270000000000001E-2</v>
       </c>
@@ -10212,7 +10220,7 @@
         <v>1.7648648648648624</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>6.7305000000000004E-2</v>
       </c>
@@ -10220,7 +10228,7 @@
         <v>1.6773648648648638</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>6.2591999999999995E-2</v>
       </c>
@@ -10228,7 +10236,7 @@
         <v>1.5922297297297328</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>5.8120999999999999E-2</v>
       </c>
@@ -10236,7 +10244,7 @@
         <v>1.5104729729729713</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>5.3884000000000001E-2</v>
       </c>
@@ -10244,7 +10252,7 @@
         <v>1.4314189189189181</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>4.9874000000000002E-2</v>
       </c>
@@ -10252,7 +10260,7 @@
         <v>1.3547297297297296</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>4.6080999999999997E-2</v>
       </c>
@@ -10260,7 +10268,7 @@
         <v>1.2814189189189205</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>4.2499000000000002E-2</v>
       </c>
@@ -10268,7 +10276,7 @@
         <v>1.2101351351351335</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>3.9119000000000001E-2</v>
       </c>
@@ -10276,7 +10284,7 @@
         <v>1.1418918918918923</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>3.5935000000000002E-2</v>
       </c>
@@ -10284,7 +10292,7 @@
         <v>1.0756756756756756</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>3.2939999999999997E-2</v>
       </c>
@@ -10292,7 +10300,7 @@
         <v>1.0118243243243259</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>3.0124999999999999E-2</v>
       </c>
@@ -10300,7 +10308,7 @@
         <v>0.95101351351351282</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2.7484999999999999E-2</v>
       </c>
@@ -10308,7 +10316,7 @@
         <v>0.89189189189189189</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2.5012E-2</v>
       </c>
@@ -10316,7 +10324,7 @@
         <v>0.83547297297297285</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2.2700999999999999E-2</v>
       </c>
@@ -10324,7 +10332,7 @@
         <v>0.7807432432432434</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2.0545000000000001E-2</v>
       </c>
@@ -10332,7 +10340,7 @@
         <v>0.72837837837837771</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>1.8537000000000001E-2</v>
       </c>
@@ -10340,7 +10348,7 @@
         <v>0.67837837837837811</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>1.6670999999999998E-2</v>
       </c>
@@ -10348,7 +10356,7 @@
         <v>0.63040540540540646</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1.4940999999999999E-2</v>
       </c>
@@ -10356,7 +10364,7 @@
         <v>0.5844594594594591</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>1.3342E-2</v>
       </c>
@@ -10364,7 +10372,7 @@
         <v>0.54020270270270254</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>1.1867000000000001E-2</v>
       </c>
@@ -10372,7 +10380,7 @@
         <v>0.49831081081081036</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1.0511E-2</v>
       </c>
@@ -10380,7 +10388,7 @@
         <v>0.45810810810810854</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>9.2680000000000002E-3</v>
       </c>
@@ -10388,7 +10396,7 @@
         <v>0.41993243243243217</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>8.1326000000000002E-3</v>
       </c>
@@ -10396,7 +10404,7 @@
         <v>0.38358108108108108</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>7.0993000000000002E-3</v>
       </c>
@@ -10404,7 +10412,7 @@
         <v>0.34908783783783781</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>6.1627000000000001E-3</v>
       </c>
@@ -10412,7 +10420,7 @@
         <v>0.31641891891891893</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>5.3175000000000002E-3</v>
       </c>
@@ -10420,7 +10428,7 @@
         <v>0.28554054054054051</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>4.5585000000000001E-3</v>
       </c>
@@ -10428,7 +10436,7 @@
         <v>0.25641891891891899</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>3.8806000000000001E-3</v>
       </c>
@@ -10436,7 +10444,7 @@
         <v>0.22902027027027022</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>3.2785000000000002E-3</v>
       </c>
@@ -10444,7 +10452,7 @@
         <v>0.20341216216216212</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2.7472999999999998E-3</v>
       </c>
@@ -10452,7 +10460,7 @@
         <v>0.17945945945945957</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2.2818999999999999E-3</v>
       </c>
@@ -10460,7 +10468,7 @@
         <v>0.15722972972972971</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>1.8775E-3</v>
       </c>
@@ -10468,7 +10476,7 @@
         <v>0.13662162162162156</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>1.5291E-3</v>
       </c>
@@ -10476,7 +10484,7 @@
         <v>0.11770270270270271</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1.2319E-3</v>
       </c>
@@ -10494,13 +10502,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18F121B-5ACB-4A52-9CC6-1BD8A79F998F}">
   <dimension ref="B1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>11</v>
       </c>
@@ -10511,7 +10519,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -10519,7 +10527,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>7</v>
       </c>
@@ -10531,7 +10539,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F4">
         <f>F3/(1000*3600)</f>
         <v>0.35555555555555557</v>
@@ -10540,7 +10548,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -10554,7 +10562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>0</f>
         <v>0</v>
@@ -10570,7 +10578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <f t="shared" ref="B7:B15" si="0">B6+0.1</f>
         <v>0.1</v>
@@ -10592,7 +10600,7 @@
         <v>0.81125358057607388</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>0.2</v>
@@ -10610,7 +10618,7 @@
         <v>808.16858508230882</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
@@ -10628,7 +10636,7 @@
         <v>805.09532105878611</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>0.4</v>
@@ -10646,7 +10654,7 @@
         <v>802.03374389356009</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>0.5</v>
@@ -10664,7 +10672,7 @@
         <v>798.98380914445511</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <f t="shared" si="0"/>
         <v>0.6</v>
@@ -10682,7 +10690,7 @@
         <v>795.94547253824078</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>0.7</v>
@@ -10700,7 +10708,7 @@
         <v>792.91868997008453</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>0.79999999999999993</v>
@@ -10718,7 +10726,7 @@
         <v>789.9034175028421</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>0.89999999999999991</v>
@@ -10736,7 +10744,7 @@
         <v>786.89961136646525</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16">
         <f>B15+0.1</f>
         <v>0.99999999999999989</v>
@@ -10754,7 +10762,7 @@
         <v>783.90722795738577</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <f t="shared" ref="B17:B31" si="4">B16+1</f>
         <v>2</v>
@@ -10772,7 +10780,7 @@
         <v>767.69733455692563</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" si="4"/>
         <v>3</v>
@@ -10790,7 +10798,7 @@
         <v>738.99825514500378</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" si="4"/>
         <v>4</v>
@@ -10808,7 +10816,7 @@
         <v>711.37204276285604</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -10826,7 +10834,7 @@
         <v>684.77859007299458</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -10844,7 +10852,7 @@
         <v>659.17928908358908</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -10862,7 +10870,7 @@
         <v>634.53697509793017</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="4"/>
         <v>8</v>
@@ -10880,7 +10888,7 @@
         <v>610.81587275927757</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -10898,7 +10906,7 @@
         <v>587.98154411269127</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -10916,7 +10924,7 @@
         <v>566.00083860851908</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -10934,7 +10942,7 @@
         <v>544.84184497489468</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -10952,7 +10960,7 @@
         <v>524.47384488942112</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -10970,7 +10978,7 @@
         <v>504.86726838275331</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -10988,7 +10996,7 @@
         <v>485.99365090932406</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -11006,7 +11014,7 @@
         <v>467.82559202295931</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -11024,7 +11032,7 @@
         <v>450.33671559727156</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32">
         <f>B31+5</f>
         <v>21</v>
@@ -11042,7 +11050,7 @@
         <v>402.27933622876009</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" ref="B33:B37" si="5">B32+5</f>
         <v>26</v>
@@ -11060,7 +11068,7 @@
         <v>332.5022787819421</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="5"/>
         <v>31</v>
@@ -11078,7 +11086,7 @@
         <v>274.82834796245851</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" si="5"/>
         <v>36</v>
@@ -11096,7 +11104,7 @@
         <v>227.1582051120549</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" si="5"/>
         <v>41</v>
@@ -11114,7 +11122,7 @@
         <v>187.75665076871562</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" si="5"/>
         <v>46</v>
@@ -11132,7 +11140,7 @@
         <v>155.18946317829798</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38">
         <f>B37+5</f>
         <v>51</v>
@@ -11150,7 +11158,7 @@
         <v>128.27119243427171</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39">
         <f>B38+10</f>
         <v>61</v>
@@ -11168,7 +11176,7 @@
         <v>96.827026245834261</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" ref="B40:B50" si="6">B39+10</f>
         <v>71</v>
@@ -11186,7 +11194,7 @@
         <v>66.15008344879972</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <f t="shared" si="6"/>
         <v>81</v>
@@ -11204,7 +11212,7 @@
         <v>45.192274408731194</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42">
         <f t="shared" si="6"/>
         <v>91</v>
@@ -11222,7 +11230,7 @@
         <v>30.874362657680418</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43">
         <f t="shared" si="6"/>
         <v>101</v>
@@ -11240,7 +11248,7 @@
         <v>21.092681923833521</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44">
         <f t="shared" si="6"/>
         <v>111</v>
@@ -11258,7 +11266,7 @@
         <v>14.410053923148395</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45">
         <f t="shared" si="6"/>
         <v>121</v>
@@ -11276,7 +11284,7 @@
         <v>9.8446302285254852</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46">
         <f t="shared" si="6"/>
         <v>131</v>
@@ -11294,7 +11302,7 @@
         <v>6.7256337036123099</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47">
         <f>B46+10</f>
         <v>141</v>
@@ -11312,7 +11320,7 @@
         <v>4.5948042399903279</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48">
         <f t="shared" si="6"/>
         <v>151</v>
@@ -11330,7 +11338,7 @@
         <v>3.139068663893152</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49">
         <f>B48+10</f>
         <v>161</v>
@@ -11348,7 +11356,7 @@
         <v>2.1445423051704871</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50">
         <f t="shared" si="6"/>
         <v>171</v>
@@ -11377,13 +11385,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249FA7AD-7E5F-4F2A-B27E-0273FE8B5239}">
   <dimension ref="B1:G81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>12</v>
       </c>
@@ -11391,7 +11399,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>13</v>
       </c>
@@ -11399,7 +11407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>14</v>
       </c>
@@ -11411,7 +11419,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F4">
         <f>F3/(3600*1000)</f>
         <v>0.75</v>
@@ -11420,7 +11428,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -11434,7 +11442,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>0</f>
         <v>0</v>
@@ -11450,7 +11458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>B6+1</f>
         <v>1</v>
@@ -11472,7 +11480,7 @@
         <v>0.28126730554493107</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" ref="B8:B31" si="1">B7+1</f>
         <v>2</v>
@@ -11494,7 +11502,7 @@
         <v>0.27950927671896558</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -11516,7 +11524,7 @@
         <v>0.2777622362492449</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -11538,7 +11546,7 @@
         <v>0.27602611545430872</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -11560,7 +11568,7 @@
         <v>0.27430084608200284</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -11582,7 +11590,7 @@
         <v>0.27258636030675243</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -11604,7 +11612,7 @@
         <v>0.27088259072693299</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -11626,7 +11634,7 @@
         <v>0.26918947036220836</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -11648,7 +11656,7 @@
         <v>0.26750693265087722</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -11670,7 +11678,7 @@
         <v>0.26583491144729077</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -11692,7 +11700,7 @@
         <v>0.26417334101923928</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -11714,7 +11722,7 @@
         <v>0.26252215604533946</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -11736,7 +11744,7 @@
         <v>0.26088129161252138</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -11758,7 +11766,7 @@
         <v>0.25925068321344058</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -11780,7 +11788,7 @@
         <v>0.25763026674392003</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -11802,7 +11810,7 @@
         <v>0.25601997850050739</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -11824,7 +11832,7 @@
         <v>0.25441975517786652</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -11846,7 +11854,7 @@
         <v>0.25282953386639995</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -11868,7 +11876,7 @@
         <v>0.25124925204966564</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -11890,7 +11898,7 @@
         <v>0.24967884760202397</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -11912,7 +11920,7 @@
         <v>0.24811825878609473</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -11934,7 +11942,7 @@
         <v>0.24656742425042399</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -11956,7 +11964,7 @@
         <v>0.24502628302699611</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -11978,7 +11986,7 @@
         <v>0.2434947745288957</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -12000,7 +12008,7 @@
         <v>0.24197283854787421</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32">
         <f>B31+5</f>
         <v>30</v>
@@ -12022,7 +12030,7 @@
         <v>0.23747320475301992</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" ref="B33:B37" si="5">B32+5</f>
         <v>35</v>
@@ -12044,7 +12052,7 @@
         <v>0.23014390680279517</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="5"/>
         <v>40</v>
@@ -12066,7 +12074,7 @@
         <v>0.22304081798845435</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" si="5"/>
         <v>45</v>
@@ -12088,7 +12096,7 @@
         <v>0.21615695666271306</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" si="5"/>
         <v>50</v>
@@ -12110,7 +12118,7 @@
         <v>0.20948555665763546</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" si="5"/>
         <v>55</v>
@@ -12132,7 +12140,7 @@
         <v>0.20302006063415978</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38">
         <f>B37+5</f>
         <v>60</v>
@@ -12154,7 +12162,7 @@
         <v>0.19675411363686313</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39">
         <f>B38+10</f>
         <v>70</v>
@@ -12176,7 +12184,7 @@
         <v>0.18773898918996673</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" ref="B40:B50" si="6">B39+10</f>
         <v>80</v>
@@ -12198,7 +12206,7 @@
         <v>0.17632918947973816</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41">
         <f t="shared" si="6"/>
         <v>90</v>
@@ -12220,7 +12228,7 @@
         <v>0.16561281807648598</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42">
         <f t="shared" si="6"/>
         <v>100</v>
@@ -12242,7 +12250,7 @@
         <v>0.15554773201283781</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43">
         <f t="shared" si="6"/>
         <v>110</v>
@@ -12264,7 +12272,7 @@
         <v>0.146094349551878</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44">
         <f t="shared" si="6"/>
         <v>120</v>
@@ -12286,7 +12294,7 @@
         <v>0.13721549452887324</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45">
         <f t="shared" si="6"/>
         <v>130</v>
@@ -12308,7 +12316,7 @@
         <v>0.128876250153107</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46">
         <f t="shared" si="6"/>
         <v>140</v>
@@ -12330,7 +12338,7 @@
         <v>0.12104382169486941</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47">
         <f>B46+10</f>
         <v>150</v>
@@ -12352,7 +12360,7 @@
         <v>0.11368740751762212</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48">
         <f t="shared" si="6"/>
         <v>160</v>
@@ -12374,7 +12382,7 @@
         <v>0.10677807794815965</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49">
         <f>B48+10</f>
         <v>170</v>
@@ -12396,7 +12404,7 @@
         <v>0.10028866150840798</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50">
         <f t="shared" si="6"/>
         <v>180</v>
@@ -12418,7 +12426,7 @@
         <v>9.4193638061466634E-2</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51">
         <f>B50+30</f>
         <v>210</v>
@@ -12440,7 +12448,7 @@
         <v>8.3201272629354478E-2</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52">
         <f t="shared" ref="B52:B81" si="7">B51+30</f>
         <v>240</v>
@@ -12462,7 +12470,7 @@
         <v>6.8934904326040505E-2</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53">
         <f t="shared" si="7"/>
         <v>270</v>
@@ -12484,7 +12492,7 @@
         <v>5.7114763804270996E-2</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54">
         <f t="shared" si="7"/>
         <v>300</v>
@@ -12506,7 +12514,7 @@
         <v>4.732140091163374E-2</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55">
         <f t="shared" si="7"/>
         <v>330</v>
@@ -12528,7 +12536,7 @@
         <v>3.9207287837406943E-2</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56">
         <f t="shared" si="7"/>
         <v>360</v>
@@ -12550,7 +12558,7 @@
         <v>3.2484486721680389E-2</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57">
         <f>B56+30</f>
         <v>390</v>
@@ -12572,7 +12580,7 @@
         <v>2.6914431876724768E-2</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58">
         <f t="shared" si="7"/>
         <v>420</v>
@@ -12594,7 +12602,7 @@
         <v>2.2299464031961987E-2</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59">
         <f t="shared" si="7"/>
         <v>450</v>
@@ -12616,7 +12624,7 @@
         <v>1.8475816186289132E-2</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60">
         <f t="shared" si="7"/>
         <v>480</v>
@@ -12638,7 +12646,7 @@
         <v>1.5307802163328844E-2</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61">
         <f t="shared" si="7"/>
         <v>510</v>
@@ -12660,7 +12668,7 @@
         <v>1.2683001644360986E-2</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62">
         <f t="shared" si="7"/>
         <v>540</v>
@@ -12682,7 +12690,7 @@
         <v>1.0508270814749192E-2</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63">
         <f t="shared" si="7"/>
         <v>570</v>
@@ -12704,7 +12712,7 @@
         <v>8.7064370574457504E-3</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64">
         <f t="shared" si="7"/>
         <v>600</v>
@@ -12726,7 +12734,7 @@
         <v>7.2135604012860573E-3</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65">
         <f t="shared" si="7"/>
         <v>630</v>
@@ -12748,7 +12756,7 @@
         <v>5.9766645436781984E-3</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66">
         <f t="shared" si="7"/>
         <v>660</v>
@@ -12770,7 +12778,7 @@
         <v>4.9518569306346814E-3</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67">
         <f t="shared" si="7"/>
         <v>690</v>
@@ -12792,7 +12800,7 @@
         <v>4.102771183203127E-3</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68">
         <f t="shared" si="7"/>
         <v>720</v>
@@ -12814,7 +12822,7 @@
         <v>3.3992765981557551E-3</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69">
         <f t="shared" si="7"/>
         <v>750</v>
@@ -12836,7 +12844,7 @@
         <v>2.8164089282084119E-3</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70">
         <f t="shared" si="7"/>
         <v>780</v>
@@ -12858,7 +12866,7 @@
         <v>2.3334844993771631E-3</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71">
         <f t="shared" si="7"/>
         <v>810</v>
@@ -12880,7 +12888,7 @@
         <v>1.9333662289933615E-3</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72">
         <f t="shared" si="7"/>
         <v>840</v>
@@ -12902,7 +12910,7 @@
         <v>1.6018554982515092E-3</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73">
         <f t="shared" si="7"/>
         <v>870</v>
@@ -12924,7 +12932,7 @@
         <v>1.327188299246653E-3</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74">
         <f t="shared" si="7"/>
         <v>900</v>
@@ -12946,7 +12954,7 @@
         <v>1.0996177767469576E-3</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75">
         <f t="shared" si="7"/>
         <v>930</v>
@@ -12968,7 +12976,7 @@
         <v>9.110683507564584E-4</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76">
         <f t="shared" si="7"/>
         <v>960</v>
@@ -12990,7 +12998,7 @@
         <v>7.5484914604205121E-4</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77">
         <f t="shared" si="7"/>
         <v>990</v>
@@ -13012,7 +13020,7 @@
         <v>6.2541655936934615E-4</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78">
         <f t="shared" si="7"/>
         <v>1020</v>
@@ -13034,7 +13042,7 @@
         <v>5.1817753889544084E-4</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79">
         <f t="shared" si="7"/>
         <v>1050</v>
@@ -13056,7 +13064,7 @@
         <v>4.2932659488020353E-4</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80">
         <f t="shared" si="7"/>
         <v>1080</v>
@@ -13078,7 +13086,7 @@
         <v>3.5571075786946192E-4</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81">
         <f t="shared" si="7"/>
         <v>1110</v>
@@ -13115,9 +13123,9 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>15</v>
       </c>
@@ -13128,7 +13136,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>16</v>
       </c>
@@ -13136,7 +13144,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>17</v>
       </c>
@@ -13148,7 +13156,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F4">
         <f>F3/(3600*1000)</f>
         <v>0.18611111111111112</v>
@@ -13157,7 +13165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -13171,7 +13179,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>0</f>
         <v>0</v>
@@ -13187,7 +13195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>B6+0.1</f>
         <v>0.1</v>
@@ -13209,7 +13217,7 @@
         <v>1.6467382558392021</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" ref="B8:B15" si="1">B7+0.1</f>
         <v>0.2</v>
@@ -13227,7 +13235,7 @@
         <v>1630.4686148745141</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" si="1"/>
         <v>0.30000000000000004</v>
@@ -13245,7 +13253,7 @@
         <v>1614.2797449450507</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <f t="shared" si="1"/>
         <v>0.4</v>
@@ -13263,7 +13271,7 @@
         <v>1598.1716460509012</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -13281,7 +13289,7 @@
         <v>1582.1443181920008</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <f t="shared" si="1"/>
         <v>0.6</v>
@@ -13299,7 +13307,7 @@
         <v>1566.1977613684128</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" si="1"/>
         <v>0.7</v>
@@ -13317,7 +13325,7 @@
         <v>1550.3319755801122</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0.79999999999999993</v>
@@ -13335,7 +13343,7 @@
         <v>1534.5469608270366</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15">
         <f t="shared" si="1"/>
         <v>0.89999999999999991</v>
@@ -13353,7 +13361,7 @@
         <v>1518.8427171092733</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16">
         <f>B15+0.1</f>
         <v>0.99999999999999989</v>
@@ -13371,7 +13379,7 @@
         <v>1503.2192444268469</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>B16+0.5</f>
         <v>1.5</v>
@@ -13389,7 +13397,7 @@
         <v>1456.9142236263331</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" ref="B18:B23" si="4">B17+0.5</f>
         <v>2</v>
@@ -13407,7 +13415,7 @@
         <v>1381.2199912723343</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" si="4"/>
         <v>2.5</v>
@@ -13425,7 +13433,7 @@
         <v>1307.5450348003233</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="4"/>
         <v>3</v>
@@ -13443,7 +13451,7 @@
         <v>1235.8893542103353</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" si="4"/>
         <v>3.5</v>
@@ -13461,7 +13469,7 @@
         <v>1166.2529495023355</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="4"/>
         <v>4</v>
@@ -13479,7 +13487,7 @@
         <v>1098.6358206763337</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="4"/>
         <v>4.5</v>
@@ -13497,7 +13505,7 @@
         <v>1033.0379677323363</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <f>B23+0.5</f>
         <v>5</v>
@@ -13515,7 +13523,7 @@
         <v>969.45939067033339</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <f>B24+0.5</f>
         <v>5.5</v>
@@ -13533,7 +13541,7 @@
         <v>907.90008949033336</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" ref="B26:B27" si="5">B25+0.5</f>
         <v>6</v>
@@ -13551,7 +13559,7 @@
         <v>848.36006419232922</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="5"/>
         <v>6.5</v>
@@ -13569,7 +13577,7 @@
         <v>790.83931477633917</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28">
         <f>B27+0.5</f>
         <v>7</v>
@@ -13587,7 +13595,7 @@
         <v>735.33784124232875</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" ref="B29:B46" si="6">B28+0.5</f>
         <v>7.5</v>
@@ -13605,7 +13613,7 @@
         <v>681.85564359033378</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="6"/>
         <v>8</v>
@@ -13623,7 +13631,7 @@
         <v>630.3927218203338</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="6"/>
         <v>8.5</v>
@@ -13641,7 +13649,7 @@
         <v>580.94907593233438</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32">
         <f t="shared" si="6"/>
         <v>9</v>
@@ -13659,7 +13667,7 @@
         <v>533.52470592633256</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" si="6"/>
         <v>9.5</v>
@@ -13677,7 +13685,7 @@
         <v>488.11961180233322</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="6"/>
         <v>10</v>
@@ -13695,7 +13703,7 @@
         <v>444.73379356033257</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" si="6"/>
         <v>10.5</v>
@@ -13713,7 +13721,7 @@
         <v>403.36725120033378</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" si="6"/>
         <v>11</v>
@@ -13731,7 +13739,7 @@
         <v>364.01998472233254</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" si="6"/>
         <v>11.5</v>
@@ -13749,7 +13757,7 @@
         <v>326.69199412633407</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38">
         <f t="shared" si="6"/>
         <v>12</v>
@@ -13767,7 +13775,7 @@
         <v>291.38327941233342</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39">
         <f t="shared" si="6"/>
         <v>12.5</v>
@@ -13785,7 +13793,7 @@
         <v>258.09384058033362</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" si="6"/>
         <v>13</v>
@@ -13803,7 +13811,7 @@
         <v>226.82367763033341</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <f t="shared" si="6"/>
         <v>13.5</v>
@@ -13821,7 +13829,7 @@
         <v>197.57279056233347</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42">
         <f t="shared" si="6"/>
         <v>14</v>
@@ -13839,7 +13847,7 @@
         <v>170.34117937633229</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43">
         <f t="shared" si="6"/>
         <v>14.5</v>
@@ -13857,7 +13865,7 @@
         <v>145.12884407233355</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44">
         <f t="shared" si="6"/>
         <v>15</v>
@@ -13875,7 +13883,7 @@
         <v>121.93578465033353</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45">
         <f t="shared" si="6"/>
         <v>15.5</v>
@@ -13893,7 +13901,7 @@
         <v>100.76200111033339</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46">
         <f t="shared" si="6"/>
         <v>16</v>
@@ -13926,9 +13934,9 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>18</v>
       </c>
@@ -13936,7 +13944,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>20</v>
       </c>
@@ -13944,7 +13952,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>21</v>
       </c>
@@ -13956,7 +13964,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F4">
         <f>F3/(3600*1000)</f>
         <v>0.19305555555555556</v>
@@ -13965,7 +13973,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -13979,7 +13987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>0</f>
         <v>0</v>
@@ -13995,7 +14003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>B6+1</f>
         <v>1</v>
@@ -14017,7 +14025,7 @@
         <v>8.4767892154311394E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" ref="B8:B31" si="1">B7+1</f>
         <v>2</v>
@@ -14039,7 +14047,7 @@
         <v>8.4147552970978146E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -14061,7 +14069,7 @@
         <v>8.3531753486491431E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -14083,7 +14091,7 @@
         <v>8.2920460478923361E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -14105,7 +14113,7 @@
         <v>8.2313640969462074E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -14127,7 +14135,7 @@
         <v>8.1711262220638264E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -14149,7 +14157,7 @@
         <v>8.1113291734563456E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -14171,7 +14179,7 @@
         <v>8.0519697251164257E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -14193,7 +14201,7 @@
         <v>7.9930446746455247E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -14215,7 +14223,7 @@
         <v>7.934550843080157E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -14237,7 +14245,7 @@
         <v>7.8764850747211179E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -14259,7 +14267,7 @@
         <v>7.8188442369625688E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -14281,7 +14289,7 @@
         <v>7.7616252201238231E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -14303,7 +14311,7 @@
         <v>7.7048249372805008E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -14325,7 +14333,7 @@
         <v>7.6484403240990123E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -14347,7 +14355,7 @@
         <v>7.5924683386710601E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -14369,7 +14377,7 @@
         <v>7.5369059613484987E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -14391,7 +14399,7 @@
         <v>7.4817501945824733E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -14413,7 +14421,7 @@
         <v>7.4269980627590521E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -14435,7 +14443,7 @@
         <v>7.3726466120413156E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -14457,7 +14465,7 @@
         <v>7.3186929102080814E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -14479,7 +14487,7 @@
         <v>7.2651340464967656E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -14501,7 +14509,7 @@
         <v>7.2119671314458386E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -14523,7 +14531,7 @@
         <v>7.1591892967390894E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -14545,7 +14553,7 @@
         <v>7.106797695051309E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32">
         <f>B31+5</f>
         <v>30</v>
@@ -14567,7 +14575,7 @@
         <v>6.9522871810997686E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" ref="B33:B37" si="5">B32+5</f>
         <v>35</v>
@@ -14589,7 +14597,7 @@
         <v>6.7015959280183626E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="5"/>
         <v>40</v>
@@ -14611,7 +14619,7 @@
         <v>6.4599443050232991E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" si="5"/>
         <v>45</v>
@@ -14633,7 +14641,7 @@
         <v>6.2270063537451438E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" si="5"/>
         <v>50</v>
@@ -14655,7 +14663,7 @@
         <v>6.0024678694877355E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" si="5"/>
         <v>55</v>
@@ -14677,7 +14685,7 @@
         <v>5.7860259774045374E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38">
         <f>B37+5</f>
         <v>60</v>
@@ -14699,7 +14707,7 @@
         <v>5.5773887239578386E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39">
         <f>B38+10</f>
         <v>70</v>
@@ -14721,7 +14729,7 @@
         <v>5.2793436299096962E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" ref="B40:B50" si="6">B39+10</f>
         <v>80</v>
@@ -14743,7 +14751,7 @@
         <v>4.9054742601845717E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41">
         <f t="shared" si="6"/>
         <v>90</v>
@@ -14765,7 +14773,7 @@
         <v>4.5580813457571791E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42">
         <f t="shared" si="6"/>
         <v>100</v>
@@ -14787,7 +14795,7 @@
         <v>4.2352898930016696E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43">
         <f t="shared" si="6"/>
         <v>110</v>
@@ -14809,7 +14817,7 @@
         <v>3.9353576904587483E-2</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44">
         <f t="shared" si="6"/>
         <v>120</v>
@@ -14831,7 +14839,7 @@
         <v>3.6566659055483841E-2</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45">
         <f t="shared" si="6"/>
         <v>130</v>
@@ -14853,7 +14861,7 @@
         <v>3.3977103471987791E-2</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46">
         <f t="shared" si="6"/>
         <v>140</v>
@@ -14875,7 +14883,7 @@
         <v>3.157093347233296E-2</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47">
         <f>B46+10</f>
         <v>150</v>
@@ -14897,7 +14905,7 @@
         <v>2.9335162166963892E-2</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48">
         <f t="shared" si="6"/>
         <v>160</v>
@@ -14919,7 +14927,7 @@
         <v>2.7257722364028642E-2</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49">
         <f>B48+10</f>
         <v>170</v>
@@ -14941,7 +14949,7 @@
         <v>2.5327401438782125E-2</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50">
         <f t="shared" si="6"/>
         <v>180</v>
@@ -14963,7 +14971,7 @@
         <v>2.3533780815368624E-2</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51">
         <f>B50+30</f>
         <v>210</v>
@@ -14985,7 +14993,7 @@
         <v>2.0355158393130783E-2</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52">
         <f t="shared" ref="B52:B75" si="7">B51+30</f>
         <v>240</v>
@@ -15007,7 +15015,7 @@
         <v>1.6329680857381415E-2</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53">
         <f t="shared" si="7"/>
         <v>270</v>
@@ -15029,7 +15037,7 @@
         <v>1.3100289948808179E-2</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54">
         <f t="shared" si="7"/>
         <v>300</v>
@@ -15051,7 +15059,7 @@
         <v>1.0509549956407698E-2</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55">
         <f t="shared" si="7"/>
         <v>330</v>
@@ -15073,7 +15081,7 @@
         <v>8.4311599756826221E-3</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56">
         <f t="shared" si="7"/>
         <v>360</v>
@@ -15095,7 +15103,7 @@
         <v>6.763796625964223E-3</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57">
         <f>B56+30</f>
         <v>390</v>
@@ -15117,7 +15125,7 @@
         <v>5.4261744444839338E-3</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58">
         <f t="shared" si="7"/>
         <v>420</v>
@@ -15139,7 +15147,7 @@
         <v>4.3530831469630856E-3</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59">
         <f t="shared" si="7"/>
         <v>450</v>
@@ -15161,7 +15169,7 @@
         <v>3.4922085676101357E-3</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60">
         <f t="shared" si="7"/>
         <v>480</v>
@@ -15183,7 +15191,7 @@
         <v>2.8015822964920448E-3</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61">
         <f t="shared" si="7"/>
         <v>510</v>
@@ -15205,7 +15213,7 @@
         <v>2.247535681807506E-3</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62">
         <f t="shared" si="7"/>
         <v>540</v>
@@ -15227,7 +15235,7 @@
         <v>1.8030584528332288E-3</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63">
         <f t="shared" si="7"/>
         <v>570</v>
@@ -15249,7 +15257,7 @@
         <v>1.4464819449357277E-3</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64">
         <f t="shared" si="7"/>
         <v>600</v>
@@ -15271,7 +15279,7 @@
         <v>1.1604227326836207E-3</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65">
         <f t="shared" si="7"/>
         <v>630</v>
@@ -15293,7 +15301,7 @@
         <v>9.3093517222488347E-4</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66">
         <f t="shared" si="7"/>
         <v>660</v>
@@ -15315,7 +15323,7 @@
         <v>7.4683153860762486E-4</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67">
         <f t="shared" si="7"/>
         <v>690</v>
@@ -15337,7 +15345,7 @@
         <v>5.9913661412751772E-4</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68">
         <f t="shared" si="7"/>
         <v>720</v>
@@ -15359,7 +15367,7 @@
         <v>4.8065013839322944E-4</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69">
         <f t="shared" si="7"/>
         <v>750</v>
@@ -15381,7 +15389,7 @@
         <v>3.855957891571304E-4</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70">
         <f t="shared" si="7"/>
         <v>780</v>
@@ -15403,7 +15411,7 @@
         <v>3.0933958141101997E-4</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71">
         <f t="shared" si="7"/>
         <v>810</v>
@@ -15425,7 +15433,7 @@
         <v>2.4816395644961474E-4</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72">
         <f t="shared" si="7"/>
         <v>840</v>
@@ -15447,7 +15455,7 @@
         <v>1.9908654754044558E-4</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73">
         <f t="shared" si="7"/>
         <v>870</v>
@@ -15469,7 +15477,7 @@
         <v>1.5971478686358306E-4</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74">
         <f t="shared" si="7"/>
         <v>900</v>
@@ -15491,7 +15499,7 @@
         <v>1.2812926567877547E-4</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75">
         <f t="shared" si="7"/>
         <v>930</v>

</xml_diff>